<commit_message>
new bug for table3
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="20475" windowHeight="9600" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -394,6 +394,18 @@
   </si>
   <si>
     <t>IE8、IE9，查询按钮不在一条直线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-2-1没有表名称，导入，报系统错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-3导出文件名不对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FileUploadDownload.xml 文件有错误。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -842,7 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1100,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1217,6 +1229,17 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1280,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1373,6 +1396,28 @@
       <c r="E5" s="5" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update buglist for 基础表管理
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -203,13 +203,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>录入数据检测是否非法
-（1）数字与字符
-（2）教工号
-（3）开始时间、结束时间的逻辑先后 表7-2-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>表6-2-4 录入失败。后台报错：
 com.microsoft.sqlserver.jdbc.SQLServerException: INSERT 语句与 FOREIGN KEY 约束"FK_T624_JuniorAdmisInfo_Admission$_DiMajorOne"冲突。该冲突发生于数据库"TDMS"，表"dbo.DiMajorOne", column 'MajorNum'。
  at cn.nit.util.DAOUtil.insert(DAOUtil.java:99)
@@ -336,10 +329,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>文件导出名称会出现乱码或者文件名超长的情况。表5、6、7可以正常导出。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>表5-1-2，导出的文件直接导入，提示错误：第5行，课程类别不存在</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -406,6 +395,123 @@
   </si>
   <si>
     <t>FileUploadDownload.xml 文件有错误。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a0c4349</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范双艳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-3-1，输入编号直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-2，1-3，1-4查询没做。输入编号，点击查询，后台报错：
+com.microsoft.sqlserver.jdbc.SQLServerException: 列名 'SeqNumber' 无效。
+ at cn.nit.dao.table1.T12DAO.totalAuditingData(T12DAO.java:60)
+ at cn.nit.service.table1.T12Service.auditingData(T12Service.java:39)
+ at cn.nit.action.table1.T12Action.auditingData(T12Action.java:99)
+ at cn.nit.util.EncodingFilter.doFilter(EncodingFilter.java:60)
+ at cn.nit.util.LoginFilter.doFilter(LoginFilter.java:37)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-5-1，1-5-2，1-7，1-8-1，1-8-2，1-8-3，1-9，没有表的名称。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-9，一打开后台就会报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表S-1-5，选择2013年数据，为空，导出报错：后台传入的数据为空。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件导出名称会出现乱码或者文件名超长的情况。表1、5、6、7可以正常导出。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>范双艳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b909150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表5-2-2，添加数据，数据合法性检查不够完善。手动输入不合法的时间，还是会录入成功。后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inpro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门管理表，没有对录入的数据合法性进行检查。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>录入数据检测是否非法
+（1）数字与字符
+（2）教工号
+（3）开始时间、结束时间的逻辑先后 表7-2-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科表，添加，需要将下拉菜单disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科表，输入编号直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发表文章类型表管理，编辑的时候文章类型代码不可编辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，添加，单位选择南昌工学院，点击保存弹出对话框“南昌工学院”，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，选择一条编辑，弹窗提示所选中的教研室号，确定之后弹窗“undefined”，选择保存弹出所属单位名称，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，选中条目点击删除，删除失败，后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学历表管理，学历名称输入为null，可以成功保存，保存之后变为空。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学位表管理，添加，输入学位代码为字母，保存成功，后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>专科专业管理，添加或编辑后无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学缘管理，还是学源管理？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -413,7 +519,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +539,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -517,7 +639,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -550,6 +672,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,16 +1013,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
     <col min="5" max="5" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -882,16 +1044,66 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -904,7 +1116,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -931,20 +1143,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="7"/>
+      <c r="D2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -954,15 +1166,17 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
     <col min="5" max="5" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -988,13 +1202,136 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="19">
+        <v>12</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1007,7 +1344,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1038,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1115,7 +1452,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1180,9 +1517,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
@@ -1191,7 +1530,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -1224,22 +1563,24 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="5">
+    <row r="10" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="19">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1252,7 +1593,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1280,20 +1621,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="7"/>
+      <c r="D2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1306,7 +1647,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1346,10 +1687,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1363,7 +1704,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="5"/>
     </row>
@@ -1372,7 +1713,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>25</v>
@@ -1380,21 +1721,21 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="54" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
+    <row r="5" spans="1:5" s="16" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1402,7 +1743,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1413,7 +1754,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1427,10 +1768,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1476,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>24</v>
@@ -1489,7 +1830,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>24</v>
@@ -1502,7 +1843,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>23</v>
@@ -1510,20 +1851,20 @@
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="D6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" ht="202.5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -1537,6 +1878,17 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1546,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1577,21 +1929,21 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>63</v>
+      <c r="D2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1599,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1610,29 +1962,35 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="6">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="14">
+        <v>5137322</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1643,29 +2001,35 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="6">
+    <row r="8" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="14">
+        <v>5137322</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1676,7 +2040,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1687,7 +2051,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1698,7 +2062,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1709,15 +2073,27 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1726,7 +2102,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1754,20 +2130,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
@@ -1796,7 +2172,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1807,7 +2183,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1818,7 +2194,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1829,7 +2205,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1840,7 +2216,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -1923,7 +2299,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -1984,7 +2360,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2013,38 +2389,38 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+      <c r="D2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>81</v>
+      <c r="E3" s="14" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -2065,14 +2441,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="97.625" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -2092,20 +2468,22 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="7"/>
+      <c r="D2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
finish test on export excel
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="255" windowWidth="20475" windowHeight="9480" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="137">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -410,10 +410,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>表4-3-1，输入编号直接回车会刷新页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>表1-2，1-3，1-4查询没做。输入编号，点击查询，后台报错：
 com.microsoft.sqlserver.jdbc.SQLServerException: 列名 'SeqNumber' 无效。
  at cn.nit.dao.table1.T12DAO.totalAuditingData(T12DAO.java:60)
@@ -440,10 +436,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>文件导出名称会出现乱码或者文件名超长的情况。表1、5、6、7可以正常导出。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>范双艳</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -461,6 +453,50 @@
   </si>
   <si>
     <t>部门管理表，没有对录入的数据合法性进行检查。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科表，添加，需要将下拉菜单disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科表，输入编号直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发表文章类型表管理，编辑的时候文章类型代码不可编辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，添加，单位选择南昌工学院，点击保存弹出对话框“南昌工学院”，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，选择一条编辑，弹窗提示所选中的教研室号，确定之后弹窗“undefined”，选择保存弹出所属单位名称，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，选中条目点击删除，删除失败，后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学历表管理，学历名称输入为null，可以成功保存，保存之后变为空。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学位表管理，添加，输入学位代码为字母，保存成功，后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>专科专业管理，添加或编辑后无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学缘管理，还是学源管理？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -471,47 +507,140 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本科表，添加，需要将下拉菜单disable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本科表，输入编号直接回车会刷新页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发表文章类型表管理，编辑的时候文章类型代码不可编辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教研室表管理，添加，单位选择南昌工学院，点击保存弹出对话框“南昌工学院”，无法保存。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教研室表管理，选择一条编辑，弹窗提示所选中的教研室号，确定之后弹窗“undefined”，选择保存弹出所属单位名称，无法保存。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教研室表管理，选中条目点击删除，删除失败，后台报错。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学历表管理，学历名称输入为null，可以成功保存，保存之后变为空。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学位表管理，添加，输入学位代码为字母，保存成功，后台报错。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>专科专业管理，添加或编辑后无法保存。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学缘管理，还是学源管理？</t>
+    <t>表2-5-2，添加，下拉菜单可以输入数据而不选择，且可以保存成功。缺乏数据合法性约束。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表2-6，添加，下拉菜单选择单位，如果再输入数字，保存会失败，后台也报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4131cc5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-2-1导出直接导入，报错：数据存储失败，请联系系统管理员。后台报错：
+不能将值 NULL 插入列 'MainClassName'，表 'TDMS.dbo.T321_MainTrainBasicInfo_Tea$'；列不允许有 Null 值。INSERT 失败。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3，审核通过数据多一行空白行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-2-2，添加数据，点击保存按钮，没有任何反应</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-3，导出表格直接导入，报错：第5行，批准设置时间格式有误（格式如：2013/02）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3ae1396</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-2-2，导出后导入（无记录的表），报错：数据存储失败，请联系管理员。后台报错：
+java.lang.ArrayIndexOutOfBoundsException: 0
+ at cn.nit.util.DAOUtil.batchInsert(DAOUtil.java:260)
+ at cn.nit.dao.table3.T322_DAO.batchInsert(T322_DAO.java:71)
+ at cn.nit.service.table3.T322_Service.batchInsert(T322_Service.java:32)
+ at cn.nit.excel.imports.table3.T322Excel.batchInsert(T322Excel.java:603)
+ at cn.nit.action.UploadAction.uploadFile(UploadAction.java:53)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-1-2，直接导出再导入，报错：数据存储失败，请联系管理员.后台报错：
+java.lang.ArrayIndexOutOfBoundsException: 0
+ at cn.nit.util.DAOUtil.batchInsert(DAOUtil.java:260)
+ at cn.nit.dao.table4.T412_Dao.batchInsert(T412_Dao.java:171)
+ at cn.nit.service.table4.T412_Service.batchInsert(T412_Service.java:38)
+ at cn.nit.excel.imports.table4.T412_Excel.batchInsert(T412_Excel.java:183)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-4-4，导出直接导入，报错：第4行，学历类别不存在。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-4-4，导出直接导入，报错：上传文件不合法。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表2-5-1，导出后直接导入数据，前台导入成功，但没有录入日期，后台报错：
+Unparseable date: "2010-05-01"
+at java.text.DateFormat.parse(DateFormat.java:337)
+at cn.nit.util.TimeUtil.changeDateYM(TimeUtil.java:83)
+at cn.nit.excel.imports.table2.T251_Excel.batchInsert(T251_Excel.java:146)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-5-2，导出后直接导入数据，前台导入成功，但没有录入日期，后台报错：
+Unparseable date: "2014-07-10"
+ at cn.nit.util.TimeUtil.changeDateYM(TimeUtil.java:83)
+ at cn.nit.excel.imports.table4.T452_Excel.batchInsert(T452_Excel.java:154)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-3-5，没有批量导入功能。表4-4-2，4-5-3可以导出后直接导入。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-1-3，4-6-1，无数据，直接导出再导入，报错：数据存储失败，请联系管理员.后台报错：
+java.lang.ArrayIndexOutOfBoundsException: 0
+ at cn.nit.util.DAOUtil.batchInsert(DAOUtil.java:260)
+ at cn.nit.dao.table4.T413_Dao.batchInsert(T413_Dao.java:190)
+ at cn.nit.service.table4.T413_Service.batchInsert(T413_Service.java:35)
+ at cn.nit.excel.imports.table4.T413_Excel.batchInsert(T413_Excel.java:325)
+java.lang.ArrayIndexOutOfBoundsException: 0
+ at cn.nit.util.DAOUtil.batchInsert(DAOUtil.java:260)
+ at cn.nit.dao.table4.T411_Dao.batchInsert(T411_Dao.java:228)
+ at cn.nit.service.table4.T411_Service.batchInsert(T411_Service.java:31)
+ at cn.nit.excel.imports.table4.T413_Excel.batchInsert(T413_Excel.java:327)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-6-1，录入非法数据（所属单位录为数字），保存，录入失败，后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-6-2，录入，数据为空，点击保存，报错：录入失败！</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-9，没有表的名称。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-3-1，输入编号直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表S4-3-6，搜索框直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表s4-6-1，s4-6-2，导出有数据，前台没有显示数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件导出名称会出现乱码或者文件名超长的情况。表1、2、3、4、5、6、7可以正常导出。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a0c4349e</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -639,7 +768,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -710,6 +839,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1066,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
@@ -1077,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
@@ -1088,7 +1226,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
@@ -1099,7 +1237,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
@@ -1168,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1215,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
@@ -1226,7 +1364,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
@@ -1237,7 +1375,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
@@ -1248,7 +1386,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -1259,7 +1397,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -1270,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
@@ -1281,7 +1419,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -1292,7 +1430,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
@@ -1303,7 +1441,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -1314,7 +1452,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
@@ -1325,11 +1463,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E13" s="21"/>
     </row>
@@ -1451,15 +1589,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1487,8 +1626,8 @@
         <v>31</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
@@ -1497,9 +1636,9 @@
       <c r="B3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
@@ -1508,22 +1647,26 @@
       <c r="B4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
@@ -1532,9 +1675,9 @@
       <c r="B6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -1543,9 +1686,9 @@
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
@@ -1554,20 +1697,20 @@
       <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19">
@@ -1576,24 +1719,25 @@
       <c r="B10" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="21"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1636,6 +1780,42 @@
       </c>
       <c r="E2" s="15"/>
     </row>
+    <row r="3" spans="1:5" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B6" s="24"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1644,10 +1824,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1738,16 +1918,22 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -1760,18 +1946,76 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
+    <row r="8" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1884,11 +2128,134 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="81" x14ac:dyDescent="0.15">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2018,7 +2385,7 @@
         <v>54</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" s="14">
         <v>5137322</v>
@@ -2084,7 +2451,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2102,7 +2469,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2178,16 +2545,22 @@
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -2233,7 +2606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2360,7 +2733,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2482,7 +2855,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update buglist for t1 t2
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="117">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -382,10 +382,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IE8、IE9，查询按钮不在一条直线</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>表3-2-1没有表名称，导入，报系统错误</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -464,54 +460,80 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>录入数据检测是否非法
+    <t>本科表，添加，需要将下拉菜单disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科表，输入编号直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发表文章类型表管理，编辑的时候文章类型代码不可编辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，添加，单位选择南昌工学院，点击保存弹出对话框“南昌工学院”，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，选择一条编辑，弹窗提示所选中的教研室号，确定之后弹窗“undefined”，选择保存弹出所属单位名称，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教研室表管理，选中条目点击删除，删除失败，后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学历表管理，学历名称输入为null，可以成功保存，保存之后变为空。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学位表管理，添加，输入学位代码为字母，保存成功，后台报错。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>专科专业管理，添加或编辑后无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学缘管理，还是学源管理？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-5-1，IE8，添加，没有显示出浏览按钮，出现的按钮无法使用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-6导出的表格，默认名称少1个括号。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>录入数据检测是否非法 表1 OK
 （1）数字与字符
 （2）教工号
 （3）开始时间、结束时间的逻辑先后 表7-2-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>本科表，添加，需要将下拉菜单disable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本科表，输入编号直接回车会刷新页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发表文章类型表管理，编辑的时候文章类型代码不可编辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教研室表管理，添加，单位选择南昌工学院，点击保存弹出对话框“南昌工学院”，无法保存。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教研室表管理，选择一条编辑，弹窗提示所选中的教研室号，确定之后弹窗“undefined”，选择保存弹出所属单位名称，无法保存。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教研室表管理，选中条目点击删除，删除失败，后台报错。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学历表管理，学历名称输入为null，可以成功保存，保存之后变为空。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学位表管理，添加，输入学位代码为字母，保存成功，后台报错。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>专科专业管理，添加或编辑后无法保存。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学缘管理，还是学源管理？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wontfix</t>
+    <t xml:space="preserve">IE8、IE9，查询按钮不在一条直线。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表2-5-1，添加数据，后台报错：
+2014-09-01 22:09:12[WARN]ognl.MethodFailedException: Method "setMachNum" failed for object cn.nit.bean.table2.T251_Bean@1cf08f [java.lang.NoSuchMethodException: cn.nit.bean.table2.T251_Bean.setMachNum([Ljava.lang.String;)]
+java.lang.NoSuchMethodException: cn.nit.bean.table2.T251_Bean.setMachNum([Ljava.lang.String;)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表2-8-5，编辑条目，如果设备台数填写为5.9，会四舍五入保存为6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1013,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1052,13 +1074,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1066,7 +1088,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
@@ -1076,22 +1098,30 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1099,11 +1129,33 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1168,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1215,7 +1267,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
@@ -1226,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
@@ -1237,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
@@ -1248,7 +1300,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -1259,7 +1311,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -1270,7 +1322,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
@@ -1281,7 +1333,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -1292,7 +1344,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
@@ -1303,7 +1355,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -1314,7 +1366,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
@@ -1325,11 +1377,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="19" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E13" s="21"/>
     </row>
@@ -1517,24 +1569,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="19">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -1563,7 +1619,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1574,26 +1630,27 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1635,6 +1692,28 @@
         <v>73</v>
       </c>
       <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1743,7 +1822,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1754,7 +1833,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1884,7 +1963,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2018,7 +2097,7 @@
         <v>54</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8" s="14">
         <v>5137322</v>
@@ -2084,7 +2163,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2482,7 +2561,7 @@
         <v>80</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update buglist for scb & hd
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="135">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,11 +62,6 @@
   </si>
   <si>
     <t>表3编辑，没有保存功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">表4-5-1，直接将导出的数据导入，提示错误：上传的文件不合法。
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -241,18 +236,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">表3-1-1，表3-1-2 添加数据保存时，后台报错
-Method "setSeqNumber" failed for object cn.nit.bean.table3.T33_Bean@1dc85da [java.lang.NoSuchMethodException: cn.nit.bean.table3.T33_Bean.setSeqNumber([Ljava.lang.String;)]
- at cn.nit.util.EncodingFilter.doFilter(EncodingFilter.java:60) 
- at cn.nit.util.LoginFilter.doFilter(LoginFilter.java:37)
-2014-07-06 16:15:29[WARN]ognl.OgnlException: target is null for setProperty(null, "SeqNumber", [Ljava.lang.String;@cd117a) </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inprocess</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>wontfix</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -361,11 +344,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">表4-1-2。条目原本齐全，选中编辑，弹出的对话框中教工号为空。出错数据（个例）：
-南昌工程学院 0000 水文与水资源工程 081102 2014000005 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>表4-1-2模版导入，使用的是insert而不是update，存在重复数据。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -403,10 +381,6 @@
   </si>
   <si>
     <t>范双艳</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表4-3-1，输入编号直接回车会刷新页面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -512,28 +486,136 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>录入数据检测是否非法 表1 OK
+    <t xml:space="preserve">IE8、IE9，查询按钮不在一条直线。 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表2-5-1，添加数据，后台报错：
+2014-09-01 22:09:12[WARN]ognl.MethodFailedException: Method "setMachNum" failed for object cn.nit.bean.table2.T251_Bean@1cf08f [java.lang.NoSuchMethodException: cn.nit.bean.table2.T251_Bean.setMachNum([Ljava.lang.String;)]
+java.lang.NoSuchMethodException: cn.nit.bean.table2.T251_Bean.setMachNum([Ljava.lang.String;)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表2-8-5，编辑条目，如果设备台数填写为5.9，会四舍五入保存为6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教学单位和所属专业没有绑定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-5-1，直接将导出的数据导入，提示错误：上传的文件不合法。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-1-2，添加，教工号下拉菜单有的教工号无法选中。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">表4-1-2。条目原本齐全，选中编辑，弹出的对话框中教工号为空。出错数据（个例）：
+南昌工程学院 0000 水文与水资源工程 081102 2014000005 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73c14a8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-2，导出的数据直接导入，后台报错：
+java.text.ParseException: Unparseable date: "2014-06-04"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-1-3，空表导入，前台报错：数据存储失败，请联系管理员。后台报错：
+java.lang.ArrayIndexOutOfBoundsException: 0
+ at cn.nit.util.DAOUtil.batchInsert(DAOUtil.java:260)
+ at cn.nit.dao.table4.T411_Dao.batchInsert(T411_Dao.java:228)
+ at cn.nit.service.table4.T411_Service.batchInsert(T411_Service.java:31)
+ at cn.nit.excel.imports.table4.T413_Excel.batchInsert(T413_Excel.java:327)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-1-1，单条添加，录入失败：
+INSERT 语句与 FOREIGN KEY 约束"FK_T411_TeaBasicInfo_Per$_DiDegree"冲突。该冲突发生于数据库"TDMS"，表"dbo.DiDegree", column 'IndexID'。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cbd43e6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-1-2，4-1-3，4-2，4-10，添加数据，录入完毕后，后台报错：
+Method "setSeqNumber" failed for object cn.nit.bean.table4.T412_Bean@1350d11
+[java.lang.NoSuchMethodException: cn.nit.bean.table4.T412_Bean.setSeqNumber([Ljava.lang.String;)]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73c14a8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-3-1，输入编号直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表s-4-3-6，输入编号直接回车会刷新页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申超波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-2-1，批量导入数据之后没有自动刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">表3-1-1，表3-1-2 添加数据保存时，后台报错
+Method "setSeqNumber" failed for object cn.nit.bean.table3.T33_Bean@1dc85da [java.lang.NoSuchMethodException: cn.nit.bean.table3.T33_Bean.setSeqNumber([Ljava.lang.String;)]
+ at cn.nit.util.EncodingFilter.doFilter(EncodingFilter.java:60) 
+ at cn.nit.util.LoginFilter.doFilter(LoginFilter.java:37)
+2014-07-06 16:15:29[WARN]ognl.OgnlException: target is null for setProperty(null, "SeqNumber", [Ljava.lang.String;@cd117a) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-1-2，单条录入，录入成功后，后台报错：
+target is null for setProperty(null, "SeqNumber", [Ljava.lang.String;@18697cd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-2-2，IE11，单条录入，如果有非法数据，不能弹窗提示，谷歌浏览器有弹窗。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-3，单条添加，批准时间和首次招生时间之间的逻辑顺序没有检查。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">表3-1-1，3-3，单条录入，保存成功，后台报错：
+Method "setSeqNumber" failed for object cn.nit.bean.table3.T311_Bean@d35396 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉框disable。表1、表2、表3、表4 OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>录入数据检测是否非法 表1 OK 表2、3、4failed
 （1）数字与字符
 （2）教工号
 （3）开始时间、结束时间的逻辑先后 表7-2-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">IE8、IE9，查询按钮不在一条直线。 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表2-5-1，添加数据，后台报错：
-2014-09-01 22:09:12[WARN]ognl.MethodFailedException: Method "setMachNum" failed for object cn.nit.bean.table2.T251_Bean@1cf08f [java.lang.NoSuchMethodException: cn.nit.bean.table2.T251_Bean.setMachNum([Ljava.lang.String;)]
-java.lang.NoSuchMethodException: cn.nit.bean.table2.T251_Bean.setMachNum([Ljava.lang.String;)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表2-8-5，编辑条目，如果设备台数填写为5.9，会四舍五入保存为6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -541,7 +623,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,6 +659,22 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -661,7 +759,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -733,6 +831,48 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1037,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1063,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1071,16 +1211,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1088,7 +1228,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
@@ -1099,10 +1239,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>4</v>
@@ -1114,10 +1254,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>4</v>
@@ -1129,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
@@ -1140,7 +1280,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
@@ -1151,7 +1291,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
@@ -1192,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1200,13 +1340,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="18"/>
     </row>
@@ -1246,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1254,10 +1394,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
@@ -1267,7 +1407,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
@@ -1278,7 +1418,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
@@ -1289,7 +1429,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
@@ -1300,7 +1440,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -1311,7 +1451,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -1322,7 +1462,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
@@ -1333,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -1344,7 +1484,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
@@ -1355,7 +1495,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -1366,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
@@ -1377,11 +1517,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C13" s="21"/>
       <c r="D13" s="19" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E13" s="21"/>
     </row>
@@ -1419,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.15">
@@ -1427,7 +1567,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1468,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1476,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1487,7 +1627,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1501,17 +1641,17 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1528,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1536,107 +1676,143 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
+      <c r="B4" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="32">
+        <v>41882</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="E6" s="29">
+        <v>41883</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19">
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="21"/>
+        <v>86</v>
+      </c>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="24">
+        <v>10</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="24"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1650,7 +1826,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1675,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1683,13 +1859,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" s="15"/>
     </row>
@@ -1698,7 +1874,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1709,7 +1885,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1723,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1752,92 +1928,161 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="33">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+    </row>
+    <row r="3" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="121.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+      <c r="C3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="32">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="27" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="B4" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" s="16" customFormat="1" ht="54" x14ac:dyDescent="0.15">
       <c r="A5" s="19">
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    </row>
+    <row r="6" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="24">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="5">
+      <c r="B6" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="32">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="24">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="32">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1847,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1858,7 +2103,7 @@
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="116" customWidth="1"/>
     <col min="3" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1875,103 +2120,192 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="33">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="35">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+      <c r="D3" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="19">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
+      <c r="B4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A5" s="24">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="19">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" ht="202.5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="5">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="24">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="81" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1980,7 +2314,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2005,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2013,16 +2347,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -2030,7 +2364,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -2041,7 +2375,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2052,10 +2386,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>4</v>
@@ -2069,7 +2403,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2080,7 +2414,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2091,13 +2425,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E8" s="14">
         <v>5137322</v>
@@ -2108,7 +2442,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2119,7 +2453,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2130,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2141,7 +2475,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2152,7 +2486,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2163,7 +2497,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2206,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2214,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>3</v>
@@ -2240,7 +2574,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2251,7 +2585,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2262,7 +2596,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2273,7 +2607,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2284,7 +2618,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2295,7 +2629,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2312,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2337,7 +2671,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.15">
@@ -2345,7 +2679,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2356,7 +2690,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2367,7 +2701,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2378,7 +2712,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2389,7 +2723,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2400,7 +2734,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2411,7 +2745,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2422,7 +2756,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2465,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2473,16 +2807,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -2490,16 +2824,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -2544,7 +2878,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -2552,16 +2886,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update buglist for fsy lhy
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" activeTab="6"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="141">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,10 +244,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>导师类别管理，导师代码可以有字符吗？添加导师信息qw qwe，后台报错</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>刘海洋</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -430,10 +426,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>部门管理表，没有对录入的数据合法性进行检查。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>本科表，添加，需要将下拉菜单disable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -608,14 +600,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>下拉框disable。表1、表2、表3、表4 OK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>录入数据检测是否非法 表1 OK 表2、3、4failed
 （1）数字与字符
 （2）教工号
 （3）开始时间、结束时间的逻辑先后 表7-2-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df7db494</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导师类别管理，导师代码可以有字符吗？添加导师信息12qasd qwe，前台报错：添加失败！后台报错：
+om.microsoft.sqlserver.jdbc.SQLServerException: 将截断字符串或二进制数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刘海洋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5bfdb2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本科表，添加之后没有自动刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门管理表，没有对录入的数据合法性进行检查。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门管理表，单位号可以有字母吗？部门名称、教工号是否做成下拉框？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉框disable。表1、表2、表3、表4、7，OK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1178,15 +1203,15 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="13.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1214,92 +1239,105 @@
         <v>11</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+      <c r="E2" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="5">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1358,18 +1396,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1389,141 +1427,205 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>138</v>
+      </c>
+      <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C8" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="19">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="19">
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" s="21"/>
+        <v>101</v>
+      </c>
+      <c r="C13" s="14"/>
       <c r="D13" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="21"/>
+        <v>102</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1644,7 +1746,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1701,10 +1803,10 @@
         <v>32</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E4" s="32">
         <v>41882</v>
@@ -1715,16 +1817,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>89</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1732,13 +1834,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E6" s="29">
         <v>41883</v>
@@ -1771,7 +1873,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1782,11 +1884,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="14"/>
     </row>
@@ -1795,7 +1897,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26" t="s">
@@ -1808,7 +1910,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1865,7 +1967,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="15"/>
     </row>
@@ -1874,7 +1976,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1885,7 +1987,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1970,7 +2072,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>24</v>
@@ -2000,7 +2102,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>24</v>
@@ -2017,7 +2119,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>24</v>
@@ -2034,7 +2136,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2045,7 +2147,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2056,7 +2158,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2067,7 +2169,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2078,7 +2180,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2128,7 +2230,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>22</v>
@@ -2145,16 +2247,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>114</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2162,16 +2264,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>114</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -2179,7 +2281,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>22</v>
@@ -2188,7 +2290,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2196,7 +2298,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>22</v>
@@ -2224,7 +2326,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>19</v>
@@ -2233,7 +2335,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
@@ -2241,7 +2343,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2252,7 +2354,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2263,7 +2365,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2274,7 +2376,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2285,7 +2387,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2296,7 +2398,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2347,16 +2449,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -2364,7 +2466,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -2375,7 +2477,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2386,10 +2488,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>4</v>
@@ -2403,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2414,7 +2516,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2425,13 +2527,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="14">
         <v>5137322</v>
@@ -2442,7 +2544,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2453,7 +2555,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2464,7 +2566,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2475,7 +2577,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2486,7 +2588,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2497,7 +2599,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2596,7 +2698,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2607,7 +2709,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2618,7 +2720,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2629,7 +2731,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2646,7 +2748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -2712,7 +2814,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2813,7 +2915,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>41</v>
@@ -2833,7 +2935,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -2892,10 +2994,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update bulist for syd
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="151">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,10 +82,6 @@
   </si>
   <si>
     <t>表7-2-1没做模版导入。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表7-3-3，直接将导出的数据导入，提示错误分为2种：（1）第4行，听课日期格式不正确，格式为：2012/09。（2）单位名称不能为空或长度不能超过100.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -632,15 +628,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>部门管理表，没有对录入的数据合法性进行检查。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>部门管理表，单位号可以有字母吗？部门名称、教工号是否做成下拉框？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>下拉框disable。表1、表2、表3、表4、7，OK</t>
+    <t>部门管理表，教工号是否做成下拉框？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0fa334d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宋亚东</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>190abc3d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表7-3-3， 单条添加，参会人数为非法数据，录入成功，后台报错：13:30:30[WARN]ognl.MethodFailedException: Method "setMeetingNum" failed for object cn.nit.bean.table7.T733_Bean@142e9fb [java.lang.NoSuchMethodException: cn.nit.bean.table7.T733_Bean.setMeetingNum([Ljava.lang.String;)]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表7-4-4，缺少数据合法性检查</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>课程类别录入的时候可以选择其他，但是批量导入的时候，如果有课程类别为其他的，就会导入失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表7-3-3，直接将导出的数据导入，提示错误分为2种：（1）第4行，听课日期格式不正确，格式为：2012/09。（2）单位名称不能为空或长度不能超过100.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表7-1-2，表7-2-2，导出的表直接导入，报错：日期格式不正确</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表7-3-2，综合评价下拉框，没有disable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉框disable。表1、表2、表3、表4，OK</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -784,7 +824,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -898,6 +938,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1203,7 +1246,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1228,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1239,13 +1282,13 @@
         <v>11</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1253,16 +1296,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.15">
@@ -1270,10 +1313,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>4</v>
@@ -1285,10 +1328,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>4</v>
@@ -1300,7 +1343,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1311,7 +1354,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1322,16 +1365,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1370,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1378,13 +1421,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="18"/>
     </row>
@@ -1398,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1424,65 +1467,75 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A2" s="33">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="B2" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="19">
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+    </row>
+    <row r="4" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="5" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="19">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1490,7 +1543,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1501,16 +1554,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -1518,16 +1571,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1535,16 +1588,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1552,7 +1605,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1563,16 +1616,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1580,16 +1633,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1597,39 +1650,50 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="5">
+    <row r="14" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="24">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="24">
+        <v>14</v>
+      </c>
+      <c r="B15" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1661,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.15">
@@ -1669,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1710,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1718,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1729,7 +1793,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1745,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1770,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
@@ -1778,7 +1842,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1789,7 +1853,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1800,13 +1864,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>123</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>124</v>
       </c>
       <c r="E4" s="32">
         <v>41882</v>
@@ -1817,16 +1881,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>87</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>88</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1834,13 +1898,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>106</v>
       </c>
       <c r="E6" s="29">
         <v>41883</v>
@@ -1851,7 +1915,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1862,7 +1926,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1873,7 +1937,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1884,11 +1948,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="14"/>
     </row>
@@ -1897,11 +1961,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" s="26"/>
       <c r="D11" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="24"/>
     </row>
@@ -1910,7 +1974,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1953,7 +2017,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1964,10 +2028,10 @@
         <v>9</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="15"/>
     </row>
@@ -1976,7 +2040,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1987,7 +2051,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2030,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
@@ -2041,13 +2105,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
@@ -2058,7 +2122,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>4</v>
@@ -2072,10 +2136,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
@@ -2085,16 +2149,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
@@ -2102,10 +2166,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>4</v>
@@ -2119,10 +2183,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>4</v>
@@ -2136,7 +2200,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2147,7 +2211,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2158,7 +2222,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2169,7 +2233,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2180,7 +2244,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2222,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
@@ -2230,10 +2294,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>4</v>
@@ -2247,16 +2311,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2264,16 +2328,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -2281,16 +2345,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2298,13 +2362,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="19"/>
     </row>
@@ -2313,10 +2377,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -2326,16 +2390,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
@@ -2343,7 +2407,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2354,7 +2418,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2365,7 +2429,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2376,7 +2440,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2387,7 +2451,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2398,7 +2462,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2441,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2449,16 +2513,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -2466,7 +2530,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -2477,7 +2541,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2488,10 +2552,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>4</v>
@@ -2505,7 +2569,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2516,7 +2580,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2527,13 +2591,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="14">
         <v>5137322</v>
@@ -2544,7 +2608,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2555,7 +2619,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2566,7 +2630,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -2577,7 +2641,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2588,7 +2652,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2599,7 +2663,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2642,7 +2706,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2650,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>3</v>
@@ -2676,7 +2740,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -2687,7 +2751,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2698,7 +2762,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2709,7 +2773,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -2720,7 +2784,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2731,7 +2795,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2746,17 +2810,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -2773,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27" x14ac:dyDescent="0.15">
@@ -2781,92 +2846,166 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+      <c r="C3" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+        <v>147</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="24">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2901,7 +3040,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -2912,13 +3051,13 @@
         <v>10</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -2926,16 +3065,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -2980,7 +3119,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -2988,16 +3127,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update for s65 t410
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="158">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -705,6 +705,10 @@
   </si>
   <si>
     <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T410，年份和数据导出不在一行。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2285,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2494,6 +2498,17 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2839,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update for scb hd fsy
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="20475" windowHeight="9570" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="195" windowWidth="20475" windowHeight="9540" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="176">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -696,10 +696,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>下拉框disable。表1、表2、表3、表4、表7，OK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>表7-1-1，在表格之外插入数据，提示系统错误，后台报错。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -709,6 +705,86 @@
   </si>
   <si>
     <t>T410，年份和数据导出不在一行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-1，6-5-2，6-5-3，6-5-4，6-5-8，导出的表直接导入，失败，报错：上传的文件不合法，后台报错：Unparseable date: "2014-08"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-5，通过率填写超过100的数字也可以成功保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5ede3dbf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f6b1a6a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表5-3-1，编辑后，会弹出对话框123.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f91beeb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表5-1-2，导出的文件直接导入，提示错误：数据存储失败，请联系管理员。后台报错：
+java.lang.ArrayIndexOutOfBoundsException: 0
+ at cn.nit.util.DAOUtil.batchInsert(DAOUtil.java:260)
+ at cn.nit.dao.table5.T512_DAO.batchInsert(T512_DAO.java:211)
+ at cn.nit.service.table5.T512_Service.batchInsert(T512_Service.java:32)
+ at cn.nit.excel.imports.table5.T512_Excel.batchInsert(T512_Excel.java:418)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉框disable。表1、表2、表3、表4、表5、表6、表7，OK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3360e06a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>46371e</t>
+  </si>
+  <si>
+    <t>表3-2-2，新版模版空表导入会报错，旧版可以提示“你导入的是空表”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-3，导出的数据直接导入，报错提示导入成功，没有自动刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-10，发表论文篇数计算错误。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-2，单条添加，无法保存。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -782,7 +858,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -846,13 +922,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -916,9 +1005,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -972,6 +1058,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1343,7 +1441,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>81</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1501,20 +1599,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A2" s="33">
+    <row r="2" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1535,20 +1633,20 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="24">
+    <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="38" t="s">
+      <c r="D4" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1601,7 +1699,7 @@
       <c r="A8" s="19">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>95</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1689,28 +1787,28 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="24">
+    <row r="14" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="23">
         <v>13</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="38" t="s">
+      <c r="D14" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="37" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="24">
+    <row r="15" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="23">
         <v>14</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>137</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -1719,7 +1817,7 @@
       <c r="D15" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E15" s="24"/>
+      <c r="E15" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1841,13 +1939,14 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1"/>
     <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1876,7 +1975,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1886,41 +1985,41 @@
       <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="24">
+    <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <v>41882</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="24">
-        <v>4</v>
-      </c>
-      <c r="B5" s="25" t="s">
+    <row r="5" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="28" t="s">
+      <c r="D5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1931,13 +2030,13 @@
       <c r="B6" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>41883</v>
       </c>
     </row>
@@ -1948,8 +2047,8 @@
       <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -1959,8 +2058,8 @@
       <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="54" x14ac:dyDescent="0.15">
@@ -1970,8 +2069,8 @@
       <c r="B9" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1981,35 +2080,41 @@
       <c r="B10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
         <v>84</v>
       </c>
       <c r="E10" s="14"/>
     </row>
-    <row r="11" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="24">
+    <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26" t="s">
+      <c r="C11" s="27"/>
+      <c r="D11" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="24"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="5">
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="40">
+        <v>41888</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2096,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2128,58 +2233,58 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="33">
+    <row r="2" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="24">
+    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="32">
+      <c r="D3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="31">
         <v>41883</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="27" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="24">
+    <row r="4" spans="1:5" s="26" customFormat="1" ht="121.5" x14ac:dyDescent="0.15">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" s="16" customFormat="1" ht="54" x14ac:dyDescent="0.15">
       <c r="A5" s="19">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -2192,37 +2297,37 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="24">
+    <row r="6" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="32">
+      <c r="D6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="31">
         <v>41883</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="24">
+    <row r="7" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="32">
+      <c r="D7" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="31">
         <v>41883</v>
       </c>
     </row>
@@ -2237,16 +2342,22 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="27" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
@@ -2259,27 +2370,57 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="5">
+    <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="5">
+      <c r="C11" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="23"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2289,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2320,20 +2461,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="33">
+    <row r="2" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="34">
         <v>41883</v>
       </c>
     </row>
@@ -2341,7 +2482,7 @@
       <c r="A3" s="19">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="19" t="s">
@@ -2371,20 +2512,20 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A5" s="24">
-        <v>4</v>
-      </c>
-      <c r="B5" s="25" t="s">
+    <row r="5" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="27" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2403,112 +2544,174 @@
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="202.5" x14ac:dyDescent="0.15">
-      <c r="A7" s="5">
+    <row r="7" spans="1:5" s="26" customFormat="1" ht="202.5" x14ac:dyDescent="0.15">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="24">
+      <c r="D7" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="31">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" s="26" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="5">
+      <c r="C9" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="31">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="5">
+      <c r="C10" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="31">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="81" x14ac:dyDescent="0.15">
-      <c r="A12" s="5">
+      <c r="C11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="31">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="26" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="5">
+      <c r="C12" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="31">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="26" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="5">
+      <c r="C13" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="31">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="23">
         <v>13</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="31">
+        <v>41888</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>157</v>
+      <c r="B15" s="35" t="s">
+        <v>156</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2519,10 +2722,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2567,27 +2770,39 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+      <c r="C3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="31">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="31">
+        <v>41888</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" s="11">
@@ -2645,16 +2860,22 @@
         <v>5137322</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
@@ -2667,49 +2888,95 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="6">
+    <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="32">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="5">
+      <c r="C11" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="5">
+      <c r="C12" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="5">
+      <c r="C13" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="23">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="41">
+        <v>14</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="81" x14ac:dyDescent="0.15">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2720,10 +2987,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2777,38 +3044,44 @@
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="5">
+    <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="128.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="30"/>
+    </row>
+    <row r="5" spans="1:5" s="26" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -2842,6 +3115,28 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2883,54 +3178,54 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A2" s="33">
+    <row r="2" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="24">
+    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="24">
+    <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="23">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2956,88 +3251,88 @@
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="24">
+    <row r="7" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="33" t="s">
+      <c r="D7" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="27" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A8" s="24">
+    <row r="8" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="33" t="s">
+      <c r="D8" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="24">
+    <row r="9" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="27" customFormat="1" ht="54" x14ac:dyDescent="0.15">
-      <c r="A10" s="24">
+    <row r="10" spans="1:5" s="26" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="24" t="s">
+      <c r="D10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="24">
+    <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="33" t="s">
+      <c r="D11" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="32" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3045,33 +3340,33 @@
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="32" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="24">
+    <row r="13" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3086,18 +3381,18 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="24">
+    <row r="15" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="23">
         <v>14</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="24"/>
+      <c r="E15" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3161,7 +3456,7 @@
       <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="14" t="s">

</xml_diff>

<commit_message>
udpate for scb hd
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="195" windowWidth="20475" windowHeight="9540" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="195" windowWidth="20475" windowHeight="9540" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="183">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -566,10 +566,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>表3-2-1，批量导入数据之后没有自动刷新。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">表3-1-1，表3-1-2 添加数据保存时，后台报错
 Method "setSeqNumber" failed for object cn.nit.bean.table3.T33_Bean@1dc85da [java.lang.NoSuchMethodException: cn.nit.bean.table3.T33_Bean.setSeqNumber([Ljava.lang.String;)]
  at cn.nit.util.EncodingFilter.doFilter(EncodingFilter.java:60) 
@@ -785,6 +781,38 @@
   </si>
   <si>
     <t>表4-2，单条添加，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国际交流与合作处，上传代码成功后，网页无响应。QQ浏览器，IE11内核。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-1-3，导出的数据直接导入，报错：第7行，学科门类错误。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-1-2，3-2-1，批量导入数据之后没有自动刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-2，单条添加，成功，后台报错：Method "setSeqNumber" failed for object cn.nit.bean.table4.T42_Bean@d68ec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>52ae02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申超波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教务处表，提交大于4M文件，前台无提示，后台报错：the request was rejected because its size (74977084) exceeds the configured maximum (2097152)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1434,7 +1462,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.15">
@@ -1503,7 +1531,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1604,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>47</v>
@@ -1613,7 +1641,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1624,13 +1652,13 @@
         <v>92</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -1638,7 +1666,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>47</v>
@@ -1647,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1658,13 +1686,13 @@
         <v>91</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1686,13 +1714,13 @@
         <v>94</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="16" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -1703,13 +1731,13 @@
         <v>95</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1720,13 +1748,13 @@
         <v>96</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1748,13 +1776,13 @@
         <v>98</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1765,13 +1793,13 @@
         <v>99</v>
       </c>
       <c r="C12" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
@@ -1792,7 +1820,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>47</v>
@@ -1801,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -1809,13 +1837,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E15" s="23"/>
     </row>
@@ -1876,17 +1904,18 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="97.625" customWidth="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
+    <col min="3" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1906,27 +1935,61 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
+    <row r="2" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="5">
+      <c r="C2" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2067,7 +2130,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -2104,7 +2167,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>49</v>
@@ -2201,10 +2264,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2272,7 +2335,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>23</v>
@@ -2336,7 +2399,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2347,7 +2410,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>23</v>
@@ -2356,7 +2419,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27" x14ac:dyDescent="0.15">
@@ -2364,7 +2427,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -2375,7 +2438,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>23</v>
@@ -2384,7 +2447,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -2392,11 +2455,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E12" s="23"/>
     </row>
@@ -2405,7 +2468,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2416,11 +2479,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2430,10 +2504,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:E13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2555,7 +2629,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" s="31">
         <v>41888</v>
@@ -2685,33 +2759,56 @@
         <v>14</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="5">
+    <row r="16" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="23">
         <v>15</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="23">
+        <v>16</v>
+      </c>
+      <c r="B17" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2725,7 +2822,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2871,10 +2968,10 @@
         <v>49</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -2899,10 +2996,10 @@
         <v>49</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -2916,10 +3013,10 @@
         <v>49</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -2933,10 +3030,10 @@
         <v>49</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -2950,10 +3047,10 @@
         <v>49</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -2961,7 +3058,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2972,7 +3069,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3053,7 +3150,7 @@
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E4" s="30"/>
     </row>
@@ -3066,7 +3163,7 @@
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E5" s="25"/>
     </row>
@@ -3079,7 +3176,7 @@
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" s="30"/>
     </row>
@@ -3121,7 +3218,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3132,7 +3229,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -3186,13 +3283,13 @@
         <v>19</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3203,13 +3300,13 @@
         <v>12</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>142</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3220,13 +3317,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="E4" s="23" t="s">
         <v>142</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.15">
@@ -3245,7 +3342,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -3259,13 +3356,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
@@ -3276,13 +3373,13 @@
         <v>20</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3293,13 +3390,13 @@
         <v>15</v>
       </c>
       <c r="C9" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="E9" s="23" t="s">
         <v>142</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="26" customFormat="1" ht="54" x14ac:dyDescent="0.15">
@@ -3307,16 +3404,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3324,16 +3421,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -3341,16 +3438,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>4</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3358,16 +3455,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="E13" s="23" t="s">
         <v>151</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -3375,7 +3472,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -3386,11 +3483,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E15" s="23"/>
     </row>

</xml_diff>

<commit_message>
update for t181-183 522
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="195" windowWidth="20475" windowHeight="9540" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="225" windowWidth="20475" windowHeight="9510" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="212">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -828,43 +828,107 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>导师类别管理表，无法删除选中条目。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑部分没有进行编码检查。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-9，不显示数据，导出的表有4条数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-6，不应有删除功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-2，学生姓名学号字段，到底是填写姓名还是学号？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-2，判断错误的逻辑顺序，与表格项目顺序不符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-2，提示的错误和实际字段不符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表T522 导出的数据跟显示的不一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T532 T534 批量导入后  页面不显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">6-1-5 不能批量导入  6-5-6 批量导入条数不对  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3134b48e5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>表1-8-1，显示只有2条数据，导出的表不止2条数据。批量导入弹窗提示“object，object”</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>导师类别管理表，无法删除选中条目。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>编辑部分没有进行编码检查。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-9，不显示数据，导出的表有4条数据。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-6，不应有删除功能。</t>
+    <t>表1-8-1，批量导入弹窗提示“object，object”，之后右下角弹窗提示数据存储成功。没有刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-8-2，1-8-3，右下角弹窗提示数据存储成功，没有刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3134b48e5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-8-1，批量导入弹窗提示“object，object”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d7ede9ea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T522，批量导入，提示没有该级别。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d3c81722</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d3c81722</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表5-1-2，显示的记录数，与实际的数目不符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b4c94388d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宋亚东</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-2，学生姓名学号字段，到底是填写姓名还是学号？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-2，判断错误的逻辑顺序，与表格项目顺序不符</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-2，提示的错误和实际字段不符</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wontfix</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1452,10 +1516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1586,23 +1650,29 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1613,11 +1683,62 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="23">
+        <v>11</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="23">
+        <v>12</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="23">
+        <v>13</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1937,7 +2058,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2280,7 +2401,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2352,7 +2473,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="25"/>
     </row>
@@ -2935,10 +3056,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3186,16 +3307,78 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="81" x14ac:dyDescent="0.15">
-      <c r="A16" s="5">
+    <row r="16" spans="1:5" s="26" customFormat="1" ht="81" x14ac:dyDescent="0.15">
+      <c r="A16" s="23">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="23">
+        <v>16</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="23">
+        <v>18</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3206,10 +3389,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3362,11 +3545,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="25"/>
     </row>
@@ -3375,11 +3558,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -3388,11 +3571,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update buglist check around
</commit_message>
<xml_diff>
--- a/buglist.xlsx
+++ b/buglist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="225" windowWidth="20475" windowHeight="9510" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="255" windowWidth="20475" windowHeight="9480" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="226">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -757,210 +757,235 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>表3-2-2，新版模版空表导入会报错，旧版可以提示“你导入的是空表”。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-3，导出的数据直接导入，报错提示导入成功，没有自动刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-10，发表论文篇数计算错误。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-2，单条添加，无法保存。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国际交流与合作处，上传代码成功后，网页无响应。QQ浏览器，IE11内核。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-1-3，导出的数据直接导入，报错：第7行，学科门类错误。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-1-2，3-2-1，批量导入数据之后没有自动刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表4-2，单条添加，成功，后台报错：Method "setSeqNumber" failed for object cn.nit.bean.table4.T42_Bean@d68ec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>52ae02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申超波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教务处表，提交大于4M文件，前台无提示，后台报错：the request was rejected because its size (74977084) exceeds the configured maximum (2097152)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申超波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5f4d64f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导师类别管理表，无法删除选中条目。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑部分没有进行编码检查。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-9，不显示数据，导出的表有4条数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-6，不应有删除功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-2，学生姓名学号字段，到底是填写姓名还是学号？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表T522 导出的数据跟显示的不一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T532 T534 批量导入后  页面不显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">6-1-5 不能批量导入  6-5-6 批量导入条数不对  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3134b48e5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-8-1，显示只有2条数据，导出的表不止2条数据。批量导入弹窗提示“object，object”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-8-1，批量导入弹窗提示“object，object”，之后右下角弹窗提示数据存储成功。没有刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-8-2，1-8-3，右下角弹窗提示数据存储成功，没有刷新。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3134b48e5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表1-8-1，批量导入弹窗提示“object，object”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d7ede9ea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T522，批量导入，提示没有该级别。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d3c81722</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d3c81722</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b4c94388d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宋亚东</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2578efc51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2578efc51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d2b2a00ec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表5-1-2，显示的记录数，与实际的数目不符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宋亚东</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74debc8a4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-6 批量导入条数不对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-2，判断错误的逻辑顺序，与表格项目顺序不符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-2，提示的错误和实际字段不符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表6-5-2，导出后导入，报错：第6行，等级不能为空。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表5-3-1，导出的表格备注一列少边框。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wontfix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>46371e</t>
-  </si>
-  <si>
-    <t>表3-2-2，新版模版空表导入会报错，旧版可以提示“你导入的是空表”。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表3-3，导出的数据直接导入，报错提示导入成功，没有自动刷新。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wontfix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表4-10，发表论文篇数计算错误。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表4-2，单条添加，无法保存。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>国际交流与合作处，上传代码成功后，网页无响应。QQ浏览器，IE11内核。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表3-1-3，导出的数据直接导入，报错：第7行，学科门类错误。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表3-1-2，3-2-1，批量导入数据之后没有自动刷新。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表4-2，单条添加，成功，后台报错：Method "setSeqNumber" failed for object cn.nit.bean.table4.T42_Bean@d68ec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>52ae02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>申超波</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>教务处表，提交大于4M文件，前台无提示，后台报错：the request was rejected because its size (74977084) exceeds the configured maximum (2097152)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>申超波</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5f4d64f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>导师类别管理表，无法删除选中条目。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>编辑部分没有进行编码检查。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-9，不显示数据，导出的表有4条数据。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-6，不应有删除功能。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-2，学生姓名学号字段，到底是填写姓名还是学号？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-2，判断错误的逻辑顺序，与表格项目顺序不符</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wontfix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表T522 导出的数据跟显示的不一样</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T532 T534 批量导入后  页面不显示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">6-1-5 不能批量导入  6-5-6 批量导入条数不对  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3134b48e5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-8-1，显示只有2条数据，导出的表不止2条数据。批量导入弹窗提示“object，object”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-8-1，批量导入弹窗提示“object，object”，之后右下角弹窗提示数据存储成功。没有刷新。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-8-2，1-8-3，右下角弹窗提示数据存储成功，没有刷新。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3134b48e5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表1-8-1，批量导入弹窗提示“object，object”</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d7ede9ea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>T522，批量导入，提示没有该级别。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d3c81722</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d3c81722</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b4c94388d</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宋亚东</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2578efc51</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2578efc51</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d2b2a00ec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表5-1-2，显示的记录数，与实际的数目不符</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宋亚东</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fixed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74debc8a4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-2，导出后导入，报错：第6行，等级不能为空。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-2，提示的错误和实际字段不符</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>表6-5-6 批量导入条数不对</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表3-2-1，导出的表格内容合并，一页之内不能找到合并的内容名称。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1554,7 +1579,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1646,16 +1671,18 @@
       </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
@@ -1690,7 +1717,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>49</v>
@@ -1699,7 +1726,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -1707,7 +1734,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>49</v>
@@ -1716,7 +1743,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -1724,7 +1751,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>49</v>
@@ -1733,7 +1760,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -1741,7 +1768,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>49</v>
@@ -1750,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -1758,7 +1785,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>49</v>
@@ -1767,7 +1794,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -1775,7 +1802,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>49</v>
@@ -1784,7 +1811,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1879,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2010,16 +2037,18 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="5">
+    <row r="10" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="19">
@@ -2105,7 +2134,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>47</v>
@@ -2114,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2158,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2177,7 +2206,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2213,13 +2242,13 @@
         <v>34</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>181</v>
-      </c>
       <c r="E2" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -2230,13 +2259,13 @@
         <v>35</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>181</v>
-      </c>
       <c r="E3" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -2244,22 +2273,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+    <row r="5" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2454,7 +2485,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2526,7 +2557,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E3" s="25"/>
     </row>
@@ -2554,10 +2585,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2684,16 +2715,22 @@
         <v>41883</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="5">
+    <row r="8" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="23">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="31">
+        <v>41898</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
       <c r="A9" s="23">
@@ -2709,19 +2746,25 @@
         <v>4</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="27" x14ac:dyDescent="0.15">
-      <c r="A10" s="5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="26" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="31">
+        <v>41898</v>
+      </c>
     </row>
     <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="23">
@@ -2758,33 +2801,56 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="5">
+    <row r="14" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="23">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="5">
+      <c r="B14" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="31">
+        <v>41898</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="23">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="B15" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="31">
+        <v>41898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2919,7 +2985,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E7" s="31">
         <v>41888</v>
@@ -3060,7 +3126,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>18</v>
@@ -3069,7 +3135,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3077,7 +3143,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>18</v>
@@ -3086,19 +3152,25 @@
         <v>4</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="23">
         <v>17</v>
       </c>
-      <c r="B18" s="35" t="s">
-        <v>178</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="40">
+        <v>41898</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3109,10 +3181,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3208,27 +3280,35 @@
         <v>5137322</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="5">
+    <row r="6" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="23">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="5">
+      <c r="C6" s="23"/>
+      <c r="D6" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6" s="40">
+        <v>41888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="23">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="40">
+        <v>41888</v>
+      </c>
     </row>
     <row r="8" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11">
@@ -3272,13 +3352,13 @@
         <v>52</v>
       </c>
       <c r="C10" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="E10" s="23" t="s">
         <v>184</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3368,13 +3448,13 @@
         <v>164</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
@@ -3382,7 +3462,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>49</v>
@@ -3391,26 +3471,32 @@
         <v>4</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="5">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="23">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="31">
+        <v>41898</v>
+      </c>
     </row>
     <row r="19" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="23">
         <v>18</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>49</v>
@@ -3419,7 +3505,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -3427,17 +3513,30 @@
         <v>19</v>
       </c>
       <c r="B20" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="E20" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>216</v>
-      </c>
+    </row>
+    <row r="21" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="23">
+        <v>20</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="E21" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3450,8 +3549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3518,7 +3617,7 @@
       </c>
       <c r="C4" s="23"/>
       <c r="D4" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="30"/>
     </row>
@@ -3576,16 +3675,20 @@
       </c>
       <c r="E8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="5">
+    <row r="9" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="23">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="23">
@@ -3622,11 +3725,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E12" s="25"/>
     </row>
@@ -3635,7 +3738,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="27"/>
@@ -3646,7 +3749,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -3657,7 +3760,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>3</v>
@@ -3672,7 +3775,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -3683,7 +3786,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -3700,8 +3803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>